<commit_message>
Updating Sub Function list
</commit_message>
<xml_diff>
--- a/Sub Function Testing.xlsx
+++ b/Sub Function Testing.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
   <si>
     <t>Setup Mode</t>
   </si>
@@ -96,9 +96,6 @@
     <t>startSampleSequence</t>
   </si>
   <si>
-    <t>Need to finalize integration</t>
-  </si>
-  <si>
     <t>Indicates the test of the sub functions in the code</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>PressureCalibration</t>
   </si>
   <si>
-    <t>Needs to be created</t>
-  </si>
-  <si>
     <t>What needs to be done</t>
   </si>
   <si>
@@ -124,6 +118,9 @@
   </si>
   <si>
     <t>How long time does it take from syringe actuation to actually melting the metal piece</t>
+  </si>
+  <si>
+    <t>More testing</t>
   </si>
 </sst>
 </file>
@@ -443,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -455,7 +452,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -567,7 +564,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -687,43 +684,43 @@
         <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
         <v>33</v>
-      </c>
-      <c r="C32" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Changes to Operation Mode and Setup Mode. Did some more testing and code seems to be working great so far!
</commit_message>
<xml_diff>
--- a/Sub Function Testing.xlsx
+++ b/Sub Function Testing.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
   <si>
     <t>Setup Mode</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>More testing</t>
+  </si>
+  <si>
+    <t>(create another script to sycn RTC?)</t>
+  </si>
+  <si>
+    <t>(false triggering?)</t>
   </si>
 </sst>
 </file>
@@ -438,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -575,7 +581,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -583,7 +589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>19</v>
       </c>
@@ -591,7 +597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>20</v>
       </c>
@@ -599,7 +605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>21</v>
       </c>
@@ -607,7 +613,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>5</v>
       </c>
@@ -615,7 +621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -623,7 +629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>4</v>
       </c>
@@ -631,7 +637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>2</v>
       </c>
@@ -639,7 +645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>6</v>
       </c>
@@ -647,7 +653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>7</v>
       </c>
@@ -655,7 +661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>8</v>
       </c>
@@ -663,7 +669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>9</v>
       </c>
@@ -671,7 +677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>10</v>
       </c>
@@ -679,7 +685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>24</v>
       </c>
@@ -687,7 +693,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>27</v>
       </c>
@@ -695,30 +701,38 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>31</v>
       </c>
       <c r="C32" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="E32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>32</v>
       </c>

</xml_diff>